<commit_message>
added FNN3 and wrote conclusion section
</commit_message>
<xml_diff>
--- a/EvaluationMatura.xlsx
+++ b/EvaluationMatura.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\stant\Desktop\ksba\MATURA\matura\matura\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\A_118784\Desktop\matura_github\matura\matura\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C68F4EB0-35E7-4251-84BF-F5F96849DDA8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A69386CA-7E6E-44A0-A85C-B7CF2B97A54C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{1FCD806C-C0A2-4BF2-8B1F-847BB30B9D6D}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{1FCD806C-C0A2-4BF2-8B1F-847BB30B9D6D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
   <si>
     <t>Total Parameters:</t>
   </si>
@@ -108,6 +108,9 @@
   </si>
   <si>
     <t>transformer4</t>
+  </si>
+  <si>
+    <t>FNN3</t>
   </si>
 </sst>
 </file>
@@ -142,7 +145,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -173,6 +176,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="14">
     <border>
@@ -440,20 +449,22 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
@@ -799,27 +810,27 @@
   <dimension ref="B2:AD32"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4:H13"/>
+      <selection activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="26.7109375" customWidth="1"/>
-    <col min="2" max="3" width="14.7109375" customWidth="1"/>
-    <col min="4" max="4" width="16.140625" customWidth="1"/>
+    <col min="1" max="1" width="26.6640625" customWidth="1"/>
+    <col min="2" max="3" width="14.6640625" customWidth="1"/>
+    <col min="4" max="4" width="16.109375" customWidth="1"/>
     <col min="5" max="5" width="15" customWidth="1"/>
-    <col min="6" max="6" width="17.42578125" customWidth="1"/>
-    <col min="7" max="7" width="17.140625" customWidth="1"/>
-    <col min="8" max="8" width="18.28515625" customWidth="1"/>
-    <col min="9" max="9" width="19.28515625" customWidth="1"/>
-    <col min="10" max="10" width="18.28515625" customWidth="1"/>
+    <col min="6" max="6" width="17.44140625" customWidth="1"/>
+    <col min="7" max="7" width="17.109375" customWidth="1"/>
+    <col min="8" max="8" width="18.33203125" customWidth="1"/>
+    <col min="9" max="9" width="19.33203125" customWidth="1"/>
+    <col min="10" max="10" width="18.33203125" customWidth="1"/>
     <col min="11" max="11" width="17" customWidth="1"/>
-    <col min="12" max="12" width="15.28515625" customWidth="1"/>
-    <col min="13" max="13" width="15.140625" customWidth="1"/>
-    <col min="14" max="14" width="15.7109375" customWidth="1"/>
+    <col min="12" max="12" width="15.33203125" customWidth="1"/>
+    <col min="13" max="13" width="15.109375" customWidth="1"/>
+    <col min="14" max="14" width="15.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:30" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:30" x14ac:dyDescent="0.3">
       <c r="D2" s="44"/>
       <c r="E2" s="44"/>
       <c r="F2" s="44"/>
@@ -829,7 +840,7 @@
       <c r="J2" s="44"/>
       <c r="K2" s="44"/>
     </row>
-    <row r="4" spans="2:30" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:30" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B4" s="12" t="s">
         <v>20</v>
       </c>
@@ -837,20 +848,23 @@
       <c r="D4" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="E4" s="21" t="s">
+      <c r="E4" s="17" t="s">
+        <v>24</v>
+      </c>
+      <c r="F4" s="21" t="s">
         <v>21</v>
       </c>
-      <c r="F4" s="17" t="s">
+      <c r="G4" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="G4" s="14" t="s">
+      <c r="H4" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="H4" s="17" t="s">
+      <c r="I4" s="17" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="2:30" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:30" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B5" s="5" t="s">
         <v>0</v>
       </c>
@@ -858,19 +872,21 @@
       <c r="D5" s="26">
         <v>6211</v>
       </c>
-      <c r="E5" s="26">
+      <c r="E5" s="48">
+        <v>8893</v>
+      </c>
+      <c r="F5" s="26">
         <v>222464</v>
       </c>
-      <c r="F5" s="26">
+      <c r="G5" s="26">
         <v>19535</v>
       </c>
-      <c r="G5" s="27">
+      <c r="H5" s="27">
         <v>114628</v>
       </c>
-      <c r="H5" s="26">
+      <c r="I5" s="26">
         <v>1494724</v>
       </c>
-      <c r="I5" s="5"/>
       <c r="O5" s="4"/>
       <c r="P5" s="4"/>
       <c r="Q5" s="4"/>
@@ -887,7 +903,7 @@
       <c r="AB5" s="1"/>
       <c r="AC5" s="1"/>
     </row>
-    <row r="6" spans="2:30" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:30" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B6" s="5" t="s">
         <v>7</v>
       </c>
@@ -895,24 +911,26 @@
       <c r="D6" s="26">
         <v>6211</v>
       </c>
-      <c r="E6" s="26" t="s">
+      <c r="E6" s="48">
+        <v>8893</v>
+      </c>
+      <c r="F6" s="26" t="s">
         <v>19</v>
       </c>
-      <c r="F6" s="26">
+      <c r="G6" s="26">
         <v>6511</v>
       </c>
-      <c r="G6" s="48">
+      <c r="H6" s="46">
         <v>38209</v>
       </c>
-      <c r="H6" s="26">
+      <c r="I6" s="26">
         <v>498241</v>
       </c>
-      <c r="I6" s="45"/>
-      <c r="J6" s="46"/>
-      <c r="K6" s="47"/>
-      <c r="L6" s="46"/>
-      <c r="M6" s="47"/>
-      <c r="N6" s="47"/>
+      <c r="J6" s="3"/>
+      <c r="K6" s="45"/>
+      <c r="L6" s="3"/>
+      <c r="M6" s="45"/>
+      <c r="N6" s="45"/>
       <c r="O6" s="4"/>
       <c r="P6" s="4"/>
       <c r="Q6" s="4"/>
@@ -929,7 +947,7 @@
       <c r="AB6" s="1"/>
       <c r="AC6" s="1"/>
     </row>
-    <row r="7" spans="2:30" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:30" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B7" s="5" t="s">
         <v>8</v>
       </c>
@@ -937,14 +955,17 @@
       <c r="D7" s="26">
         <v>0</v>
       </c>
-      <c r="E7" s="26"/>
-      <c r="F7" s="26">
+      <c r="E7" s="48">
+        <v>0</v>
+      </c>
+      <c r="F7" s="26"/>
+      <c r="G7" s="26">
         <v>13024</v>
       </c>
-      <c r="G7" s="27">
+      <c r="H7" s="27">
         <v>76419</v>
       </c>
-      <c r="H7" s="26">
+      <c r="I7" s="26">
         <v>996483</v>
       </c>
       <c r="M7" s="4"/>
@@ -965,7 +986,7 @@
       <c r="AB7" s="1"/>
       <c r="AC7" s="1"/>
     </row>
-    <row r="8" spans="2:30" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:30" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B8" s="6" t="s">
         <v>1</v>
       </c>
@@ -973,16 +994,19 @@
       <c r="D8" s="15">
         <v>3.8940559999999999E-2</v>
       </c>
-      <c r="E8" s="15">
+      <c r="E8" s="7">
+        <v>3.4600346999999997E-2</v>
+      </c>
+      <c r="F8" s="15">
         <v>0.27306467000000001</v>
       </c>
-      <c r="F8" s="15">
+      <c r="G8" s="15">
         <v>0.59083264999999996</v>
       </c>
-      <c r="G8" s="22">
+      <c r="H8" s="22">
         <v>4.4807515999999999E-2</v>
       </c>
-      <c r="H8" s="18">
+      <c r="I8" s="18">
         <v>3.8198325999999998E-2</v>
       </c>
       <c r="M8" s="3"/>
@@ -1004,7 +1028,7 @@
       <c r="AC8" s="3"/>
       <c r="AD8" s="3"/>
     </row>
-    <row r="9" spans="2:30" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:30" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B9" s="6" t="s">
         <v>2</v>
       </c>
@@ -1012,16 +1036,19 @@
       <c r="D9" s="15">
         <v>1.5550438999999999E-2</v>
       </c>
-      <c r="E9" s="15">
+      <c r="E9" s="7">
+        <v>1.3437587000000001E-2</v>
+      </c>
+      <c r="F9" s="15">
         <v>0.11351999</v>
       </c>
-      <c r="F9" s="15">
+      <c r="G9" s="15">
         <v>0.27122992000000001</v>
       </c>
-      <c r="G9" s="22">
+      <c r="H9" s="22">
         <v>1.8804727E-2</v>
       </c>
-      <c r="H9" s="18">
+      <c r="I9" s="18">
         <v>1.5183598E-2</v>
       </c>
       <c r="M9" s="3"/>
@@ -1043,7 +1070,7 @@
       <c r="AC9" s="3"/>
       <c r="AD9" s="3"/>
     </row>
-    <row r="10" spans="2:30" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:30" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B10" s="34" t="s">
         <v>3</v>
       </c>
@@ -1051,16 +1078,19 @@
       <c r="D10" s="36">
         <v>2.2301364000000001</v>
       </c>
-      <c r="E10" s="36">
+      <c r="E10" s="49">
+        <v>2.5046073999999998</v>
+      </c>
+      <c r="F10" s="36">
         <v>3.5727410000000002</v>
       </c>
-      <c r="F10" s="36">
+      <c r="G10" s="36">
         <v>3.2350099999999999</v>
       </c>
-      <c r="G10" s="38">
+      <c r="H10" s="38">
         <v>4.5702313999999999</v>
       </c>
-      <c r="H10" s="37">
+      <c r="I10" s="37">
         <v>4.9287004000000003</v>
       </c>
       <c r="M10" s="3"/>
@@ -1082,7 +1112,7 @@
       <c r="AC10" s="3"/>
       <c r="AD10" s="3"/>
     </row>
-    <row r="11" spans="2:30" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:30" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B11" s="34" t="s">
         <v>4</v>
       </c>
@@ -1090,16 +1120,19 @@
       <c r="D11" s="36">
         <v>0.25092703</v>
       </c>
-      <c r="E11" s="36">
+      <c r="E11" s="49">
+        <v>0.2908847</v>
+      </c>
+      <c r="F11" s="36">
         <v>0.34720424</v>
       </c>
-      <c r="F11" s="36">
+      <c r="G11" s="36">
         <v>0.34040624000000003</v>
       </c>
-      <c r="G11" s="38">
+      <c r="H11" s="38">
         <v>0.52014590000000005</v>
       </c>
-      <c r="H11" s="37">
+      <c r="I11" s="37">
         <v>0.54311573999999996</v>
       </c>
       <c r="M11" s="3"/>
@@ -1121,7 +1154,7 @@
       <c r="AC11" s="3"/>
       <c r="AD11" s="3"/>
     </row>
-    <row r="12" spans="2:30" s="2" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:30" s="2" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B12" s="8" t="s">
         <v>5</v>
       </c>
@@ -1129,16 +1162,19 @@
       <c r="D12" s="16">
         <v>6.2929915999999997</v>
       </c>
-      <c r="E12" s="16">
+      <c r="E12" s="9">
+        <v>6.1168722999999998</v>
+      </c>
+      <c r="F12" s="16">
         <v>6.0766929999999997</v>
       </c>
-      <c r="F12" s="16">
+      <c r="G12" s="16">
         <v>2.7806435</v>
       </c>
-      <c r="G12" s="23">
+      <c r="H12" s="23">
         <v>6.1630589999999996</v>
       </c>
-      <c r="H12" s="19">
+      <c r="I12" s="19">
         <v>6.0680326999999998</v>
       </c>
       <c r="M12" s="3"/>
@@ -1160,7 +1196,7 @@
       <c r="AC12" s="3"/>
       <c r="AD12" s="3"/>
     </row>
-    <row r="13" spans="2:30" s="2" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:30" s="2" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B13" s="10" t="s">
         <v>6</v>
       </c>
@@ -1168,16 +1204,19 @@
       <c r="D13" s="25">
         <v>6.6345832323533598</v>
       </c>
-      <c r="E13" s="24">
+      <c r="E13" s="50">
+        <v>6.6725211721686204</v>
+      </c>
+      <c r="F13" s="24">
         <v>0.47937871630182899</v>
       </c>
-      <c r="F13" s="25">
+      <c r="G13" s="25">
         <v>1.7374969</v>
       </c>
-      <c r="G13" s="24">
+      <c r="H13" s="24">
         <v>2.8882827192635498</v>
       </c>
-      <c r="H13" s="24">
+      <c r="I13" s="24">
         <v>5.2896367793635601</v>
       </c>
       <c r="M13" s="3"/>
@@ -1199,7 +1238,7 @@
       <c r="AC13" s="3"/>
       <c r="AD13" s="3"/>
     </row>
-    <row r="17" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B17" s="12" t="s">
         <v>22</v>
       </c>
@@ -1214,7 +1253,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="18" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B18" s="41" t="s">
         <v>15</v>
       </c>
@@ -1228,7 +1267,7 @@
         <v>270000000</v>
       </c>
     </row>
-    <row r="19" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B19" s="30" t="s">
         <v>10</v>
       </c>
@@ -1243,7 +1282,7 @@
         <v>54.22</v>
       </c>
     </row>
-    <row r="20" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B20" s="31" t="s">
         <v>11</v>
       </c>
@@ -1258,7 +1297,7 @@
         <v>9.67</v>
       </c>
     </row>
-    <row r="21" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B21" s="39" t="s">
         <v>12</v>
       </c>
@@ -1273,29 +1312,27 @@
         <v>28</v>
       </c>
     </row>
-    <row r="30" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="H30" s="49"/>
-      <c r="I30" s="50"/>
-      <c r="J30" s="50"/>
-      <c r="K30" s="50"/>
-      <c r="L30" s="50"/>
-      <c r="M30" s="50"/>
-    </row>
-    <row r="31" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="H31" s="49"/>
-      <c r="I31" s="45"/>
-      <c r="J31" s="45"/>
-      <c r="K31" s="45"/>
-      <c r="L31" s="45"/>
-      <c r="M31" s="45"/>
-    </row>
-    <row r="32" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="H32" s="45"/>
-      <c r="I32" s="46"/>
-      <c r="J32" s="46"/>
-      <c r="K32" s="46"/>
-      <c r="L32" s="47"/>
-      <c r="M32" s="47"/>
+    <row r="30" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="I30" s="47"/>
+      <c r="J30" s="47"/>
+      <c r="K30" s="47"/>
+      <c r="L30" s="47"/>
+      <c r="M30" s="47"/>
+    </row>
+    <row r="31" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="I31" s="2"/>
+      <c r="J31" s="2"/>
+      <c r="K31" s="2"/>
+      <c r="L31" s="2"/>
+      <c r="M31" s="2"/>
+    </row>
+    <row r="32" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="H32" s="2"/>
+      <c r="I32" s="3"/>
+      <c r="J32" s="3"/>
+      <c r="K32" s="3"/>
+      <c r="L32" s="45"/>
+      <c r="M32" s="45"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
added future work, wrote some more in findings.
</commit_message>
<xml_diff>
--- a/EvaluationMatura.xlsx
+++ b/EvaluationMatura.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\A_118784\Desktop\matura_github\matura\matura\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A69386CA-7E6E-44A0-A85C-B7CF2B97A54C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E3AAE15-C930-4E5B-BE18-573C7C1F94D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{1FCD806C-C0A2-4BF2-8B1F-847BB30B9D6D}"/>
   </bookViews>
@@ -349,7 +349,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="51">
+  <cellXfs count="52">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -467,6 +467,7 @@
     <xf numFmtId="164" fontId="0" fillId="3" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -809,7 +810,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D91AE2C6-BFCA-42B0-A11A-AEC485B0CB91}">
   <dimension ref="B2:AD32"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
@@ -958,7 +959,9 @@
       <c r="E7" s="48">
         <v>0</v>
       </c>
-      <c r="F7" s="26"/>
+      <c r="F7" s="26">
+        <v>0</v>
+      </c>
       <c r="G7" s="26">
         <v>13024</v>
       </c>
@@ -1252,6 +1255,7 @@
       <c r="F17" s="17" t="s">
         <v>13</v>
       </c>
+      <c r="H17" s="51"/>
     </row>
     <row r="18" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B18" s="41" t="s">

</xml_diff>

<commit_message>
added changes to excel and tofindings and methodology. not finished
</commit_message>
<xml_diff>
--- a/EvaluationMatura.xlsx
+++ b/EvaluationMatura.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\A_118784\Desktop\matura_github\matura\matura\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\stant\Desktop\ksba\MATURA\matura\matura\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E3AAE15-C930-4E5B-BE18-573C7C1F94D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE7C1119-7055-4F16-B216-FA251BFC199E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{1FCD806C-C0A2-4BF2-8B1F-847BB30B9D6D}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{1FCD806C-C0A2-4BF2-8B1F-847BB30B9D6D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
   <si>
     <t>Total Parameters:</t>
   </si>
@@ -111,19 +111,23 @@
   </si>
   <si>
     <t>FNN3</t>
+  </si>
+  <si>
+    <t>Benchmark score p-value:</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="4">
+  <numFmts count="5">
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="164" formatCode="0.000000"/>
     <numFmt numFmtId="165" formatCode="0.0000000"/>
     <numFmt numFmtId="166" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="172" formatCode="0.000"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -144,8 +148,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -182,8 +192,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="14">
+  <borders count="16">
     <border>
       <left/>
       <right/>
@@ -339,6 +355,30 @@
       </left>
       <right/>
       <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
       <bottom style="thin">
         <color indexed="64"/>
       </bottom>
@@ -349,7 +389,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="52">
+  <cellXfs count="55">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -387,34 +427,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="4" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="165" fontId="1" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="165" fontId="1" fillId="4" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="1" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="165" fontId="1" fillId="4" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="165" fontId="1" fillId="3" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="3" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -434,15 +450,6 @@
     <xf numFmtId="164" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="5" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="165" fontId="1" fillId="5" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="165" fontId="1" fillId="5" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -468,6 +475,42 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="172" fontId="0" fillId="7" borderId="15" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="5" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="5" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="4" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="4" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="3" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -810,38 +853,38 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D91AE2C6-BFCA-42B0-A11A-AEC485B0CB91}">
   <dimension ref="B2:AD32"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H17" sqref="H17"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J20" sqref="J20:J21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="26.6640625" customWidth="1"/>
-    <col min="2" max="3" width="14.6640625" customWidth="1"/>
-    <col min="4" max="4" width="16.109375" customWidth="1"/>
+    <col min="1" max="1" width="26.7109375" customWidth="1"/>
+    <col min="2" max="3" width="14.7109375" customWidth="1"/>
+    <col min="4" max="4" width="16.140625" customWidth="1"/>
     <col min="5" max="5" width="15" customWidth="1"/>
-    <col min="6" max="6" width="17.44140625" customWidth="1"/>
-    <col min="7" max="7" width="17.109375" customWidth="1"/>
-    <col min="8" max="8" width="18.33203125" customWidth="1"/>
-    <col min="9" max="9" width="19.33203125" customWidth="1"/>
-    <col min="10" max="10" width="18.33203125" customWidth="1"/>
+    <col min="6" max="6" width="17.42578125" customWidth="1"/>
+    <col min="7" max="7" width="17.140625" customWidth="1"/>
+    <col min="8" max="8" width="18.28515625" customWidth="1"/>
+    <col min="9" max="9" width="19.28515625" customWidth="1"/>
+    <col min="10" max="10" width="18.28515625" customWidth="1"/>
     <col min="11" max="11" width="17" customWidth="1"/>
-    <col min="12" max="12" width="15.33203125" customWidth="1"/>
-    <col min="13" max="13" width="15.109375" customWidth="1"/>
-    <col min="14" max="14" width="15.6640625" customWidth="1"/>
+    <col min="12" max="12" width="15.28515625" customWidth="1"/>
+    <col min="13" max="13" width="15.140625" customWidth="1"/>
+    <col min="14" max="14" width="15.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:30" x14ac:dyDescent="0.3">
-      <c r="D2" s="44"/>
-      <c r="E2" s="44"/>
-      <c r="F2" s="44"/>
-      <c r="G2" s="44"/>
-      <c r="H2" s="44"/>
-      <c r="I2" s="44"/>
-      <c r="J2" s="44"/>
-      <c r="K2" s="44"/>
-    </row>
-    <row r="4" spans="2:30" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:30" x14ac:dyDescent="0.25">
+      <c r="D2" s="33"/>
+      <c r="E2" s="33"/>
+      <c r="F2" s="33"/>
+      <c r="G2" s="33"/>
+      <c r="H2" s="33"/>
+      <c r="I2" s="33"/>
+      <c r="J2" s="33"/>
+      <c r="K2" s="33"/>
+    </row>
+    <row r="4" spans="2:30" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="12" t="s">
         <v>20</v>
       </c>
@@ -849,43 +892,43 @@
       <c r="D4" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="E4" s="17" t="s">
+      <c r="E4" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="F4" s="21" t="s">
+      <c r="F4" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="G4" s="17" t="s">
+      <c r="G4" s="15" t="s">
         <v>17</v>
       </c>
       <c r="H4" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="I4" s="17" t="s">
+      <c r="I4" s="15" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="2:30" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:30" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B5" s="5" t="s">
         <v>0</v>
       </c>
       <c r="C5" s="4"/>
-      <c r="D5" s="26">
+      <c r="D5" s="18">
         <v>6211</v>
       </c>
-      <c r="E5" s="48">
+      <c r="E5" s="37">
         <v>8893</v>
       </c>
-      <c r="F5" s="26">
+      <c r="F5" s="18">
         <v>222464</v>
       </c>
-      <c r="G5" s="26">
+      <c r="G5" s="18">
         <v>19535</v>
       </c>
-      <c r="H5" s="27">
+      <c r="H5" s="19">
         <v>114628</v>
       </c>
-      <c r="I5" s="26">
+      <c r="I5" s="18">
         <v>1494724</v>
       </c>
       <c r="O5" s="4"/>
@@ -904,34 +947,34 @@
       <c r="AB5" s="1"/>
       <c r="AC5" s="1"/>
     </row>
-    <row r="6" spans="2:30" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:30" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B6" s="5" t="s">
         <v>7</v>
       </c>
       <c r="C6" s="4"/>
-      <c r="D6" s="26">
+      <c r="D6" s="18">
         <v>6211</v>
       </c>
-      <c r="E6" s="48">
+      <c r="E6" s="37">
         <v>8893</v>
       </c>
-      <c r="F6" s="26" t="s">
+      <c r="F6" s="18" t="s">
         <v>19</v>
       </c>
-      <c r="G6" s="26">
+      <c r="G6" s="18">
         <v>6511</v>
       </c>
-      <c r="H6" s="46">
+      <c r="H6" s="35">
         <v>38209</v>
       </c>
-      <c r="I6" s="26">
+      <c r="I6" s="18">
         <v>498241</v>
       </c>
       <c r="J6" s="3"/>
-      <c r="K6" s="45"/>
+      <c r="K6" s="34"/>
       <c r="L6" s="3"/>
-      <c r="M6" s="45"/>
-      <c r="N6" s="45"/>
+      <c r="M6" s="34"/>
+      <c r="N6" s="34"/>
       <c r="O6" s="4"/>
       <c r="P6" s="4"/>
       <c r="Q6" s="4"/>
@@ -948,27 +991,27 @@
       <c r="AB6" s="1"/>
       <c r="AC6" s="1"/>
     </row>
-    <row r="7" spans="2:30" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:30" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B7" s="5" t="s">
         <v>8</v>
       </c>
       <c r="C7" s="4"/>
-      <c r="D7" s="26">
+      <c r="D7" s="18">
         <v>0</v>
       </c>
-      <c r="E7" s="48">
+      <c r="E7" s="37">
         <v>0</v>
       </c>
-      <c r="F7" s="26">
+      <c r="F7" s="18">
         <v>0</v>
       </c>
-      <c r="G7" s="26">
+      <c r="G7" s="18">
         <v>13024</v>
       </c>
-      <c r="H7" s="27">
+      <c r="H7" s="19">
         <v>76419</v>
       </c>
-      <c r="I7" s="26">
+      <c r="I7" s="18">
         <v>996483</v>
       </c>
       <c r="M7" s="4"/>
@@ -989,28 +1032,28 @@
       <c r="AB7" s="1"/>
       <c r="AC7" s="1"/>
     </row>
-    <row r="8" spans="2:30" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:30" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B8" s="6" t="s">
         <v>1</v>
       </c>
       <c r="C8" s="7"/>
-      <c r="D8" s="15">
-        <v>3.8940559999999999E-2</v>
+      <c r="D8" s="45">
+        <v>2.6853999999999999E-2</v>
       </c>
       <c r="E8" s="7">
-        <v>3.4600346999999997E-2</v>
-      </c>
-      <c r="F8" s="15">
-        <v>0.27306467000000001</v>
-      </c>
-      <c r="G8" s="15">
-        <v>0.59083264999999996</v>
-      </c>
-      <c r="H8" s="22">
-        <v>4.4807515999999999E-2</v>
-      </c>
-      <c r="I8" s="18">
-        <v>3.8198325999999998E-2</v>
+        <v>2.7486E-2</v>
+      </c>
+      <c r="F8" s="45">
+        <v>0.24498</v>
+      </c>
+      <c r="G8" s="45">
+        <v>0.81411263700945302</v>
+      </c>
+      <c r="H8" s="46">
+        <v>3.9309111613890203E-2</v>
+      </c>
+      <c r="I8" s="47">
+        <v>3.65881556991485E-2</v>
       </c>
       <c r="M8" s="3"/>
       <c r="N8" s="3"/>
@@ -1031,28 +1074,28 @@
       <c r="AC8" s="3"/>
       <c r="AD8" s="3"/>
     </row>
-    <row r="9" spans="2:30" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:30" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B9" s="6" t="s">
         <v>2</v>
       </c>
       <c r="C9" s="7"/>
-      <c r="D9" s="15">
-        <v>1.5550438999999999E-2</v>
+      <c r="D9" s="45">
+        <v>1.0966E-2</v>
       </c>
       <c r="E9" s="7">
-        <v>1.3437587000000001E-2</v>
-      </c>
-      <c r="F9" s="15">
-        <v>0.11351999</v>
-      </c>
-      <c r="G9" s="15">
-        <v>0.27122992000000001</v>
-      </c>
-      <c r="H9" s="22">
-        <v>1.8804727E-2</v>
-      </c>
-      <c r="I9" s="18">
-        <v>1.5183598E-2</v>
+        <v>1.1122E-2</v>
+      </c>
+      <c r="F9" s="45">
+        <v>9.3975000000000003E-2</v>
+      </c>
+      <c r="G9" s="45">
+        <v>0.302951403012997</v>
+      </c>
+      <c r="H9" s="46">
+        <v>1.63185627726859E-2</v>
+      </c>
+      <c r="I9" s="47">
+        <v>1.4935819183805101E-2</v>
       </c>
       <c r="M9" s="3"/>
       <c r="N9" s="3"/>
@@ -1073,28 +1116,28 @@
       <c r="AC9" s="3"/>
       <c r="AD9" s="3"/>
     </row>
-    <row r="10" spans="2:30" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="34" t="s">
+    <row r="10" spans="2:30" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B10" s="26" t="s">
         <v>3</v>
       </c>
-      <c r="C10" s="35"/>
-      <c r="D10" s="36">
-        <v>2.2301364000000001</v>
-      </c>
-      <c r="E10" s="49">
-        <v>2.5046073999999998</v>
-      </c>
-      <c r="F10" s="36">
-        <v>3.5727410000000002</v>
-      </c>
-      <c r="G10" s="36">
-        <v>3.2350099999999999</v>
-      </c>
-      <c r="H10" s="38">
-        <v>4.5702313999999999</v>
-      </c>
-      <c r="I10" s="37">
-        <v>4.9287004000000003</v>
+      <c r="C10" s="27"/>
+      <c r="D10" s="48">
+        <v>2.1783429999999999</v>
+      </c>
+      <c r="E10" s="38">
+        <v>2.3717000000000001</v>
+      </c>
+      <c r="F10" s="48">
+        <v>3.7376680000000002</v>
+      </c>
+      <c r="G10" s="48">
+        <v>3.9705149551023999</v>
+      </c>
+      <c r="H10" s="49">
+        <v>4.4195793066857698</v>
+      </c>
+      <c r="I10" s="50">
+        <v>4.9018877277559101</v>
       </c>
       <c r="M10" s="3"/>
       <c r="N10" s="3"/>
@@ -1115,28 +1158,28 @@
       <c r="AC10" s="3"/>
       <c r="AD10" s="3"/>
     </row>
-    <row r="11" spans="2:30" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="34" t="s">
+    <row r="11" spans="2:30" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="26" t="s">
         <v>4</v>
       </c>
-      <c r="C11" s="35"/>
-      <c r="D11" s="36">
-        <v>0.25092703</v>
-      </c>
-      <c r="E11" s="49">
-        <v>0.2908847</v>
-      </c>
-      <c r="F11" s="36">
-        <v>0.34720424</v>
-      </c>
-      <c r="G11" s="36">
-        <v>0.34040624000000003</v>
-      </c>
-      <c r="H11" s="38">
-        <v>0.52014590000000005</v>
-      </c>
-      <c r="I11" s="37">
-        <v>0.54311573999999996</v>
+      <c r="C11" s="27"/>
+      <c r="D11" s="48">
+        <v>0.250031</v>
+      </c>
+      <c r="E11" s="38">
+        <v>0.27529900000000002</v>
+      </c>
+      <c r="F11" s="48">
+        <v>0.36363000000000001</v>
+      </c>
+      <c r="G11" s="48">
+        <v>0.43386028035445201</v>
+      </c>
+      <c r="H11" s="49">
+        <v>0.49537660469524197</v>
+      </c>
+      <c r="I11" s="50">
+        <v>0.53989104243156505</v>
       </c>
       <c r="M11" s="3"/>
       <c r="N11" s="3"/>
@@ -1157,28 +1200,28 @@
       <c r="AC11" s="3"/>
       <c r="AD11" s="3"/>
     </row>
-    <row r="12" spans="2:30" s="2" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="2:30" s="2" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B12" s="8" t="s">
         <v>5</v>
       </c>
       <c r="C12" s="9"/>
-      <c r="D12" s="16">
-        <v>6.2929915999999997</v>
+      <c r="D12" s="51">
+        <v>6.1556709999999999</v>
       </c>
       <c r="E12" s="9">
-        <v>6.1168722999999998</v>
-      </c>
-      <c r="F12" s="16">
-        <v>6.0766929999999997</v>
-      </c>
-      <c r="G12" s="16">
-        <v>2.7806435</v>
-      </c>
-      <c r="H12" s="23">
-        <v>6.1630589999999996</v>
-      </c>
-      <c r="I12" s="19">
-        <v>6.0680326999999998</v>
+        <v>5.6474900000000003</v>
+      </c>
+      <c r="F12" s="51">
+        <v>5.5192399999999999</v>
+      </c>
+      <c r="G12" s="51">
+        <v>2.9318039763569801</v>
+      </c>
+      <c r="H12" s="52">
+        <v>3.8864000312505</v>
+      </c>
+      <c r="I12" s="53">
+        <v>3.8015068469047502</v>
       </c>
       <c r="M12" s="3"/>
       <c r="N12" s="3"/>
@@ -1199,28 +1242,28 @@
       <c r="AC12" s="3"/>
       <c r="AD12" s="3"/>
     </row>
-    <row r="13" spans="2:30" s="2" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="2:30" s="2" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B13" s="10" t="s">
         <v>6</v>
       </c>
       <c r="C13" s="11"/>
-      <c r="D13" s="25">
-        <v>6.6345832323533598</v>
-      </c>
-      <c r="E13" s="50">
-        <v>6.6725211721686204</v>
-      </c>
-      <c r="F13" s="24">
-        <v>0.47937871630182899</v>
-      </c>
-      <c r="G13" s="25">
-        <v>1.7374969</v>
-      </c>
-      <c r="H13" s="24">
-        <v>2.8882827192635498</v>
-      </c>
-      <c r="I13" s="24">
-        <v>5.2896367793635601</v>
+      <c r="D13" s="39">
+        <v>10.702839000000001</v>
+      </c>
+      <c r="E13" s="39">
+        <v>8.9083310000000004</v>
+      </c>
+      <c r="F13" s="54">
+        <v>0.66537000000000002</v>
+      </c>
+      <c r="G13" s="39">
+        <v>2.2023795683112599</v>
+      </c>
+      <c r="H13" s="54">
+        <v>5.0238834103101597</v>
+      </c>
+      <c r="I13" s="54">
+        <v>4.77111888103199</v>
       </c>
       <c r="M13" s="3"/>
       <c r="N13" s="3"/>
@@ -1241,102 +1284,130 @@
       <c r="AC13" s="3"/>
       <c r="AD13" s="3"/>
     </row>
-    <row r="17" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:30" x14ac:dyDescent="0.25">
+      <c r="B14" s="42" t="s">
+        <v>25</v>
+      </c>
+      <c r="C14" s="43"/>
+      <c r="D14" s="44">
+        <v>6.7999999999999999E-5</v>
+      </c>
+      <c r="E14" s="44">
+        <v>6.2000000000000003E-5</v>
+      </c>
+      <c r="F14" s="44">
+        <v>4.75E-4</v>
+      </c>
+      <c r="G14" s="44">
+        <v>0.13441415336853399</v>
+      </c>
+      <c r="H14" s="44">
+        <v>2.6458572938701601E-3</v>
+      </c>
+      <c r="I14" s="44">
+        <v>1.19961547549787E-2</v>
+      </c>
+      <c r="J14" s="30"/>
+    </row>
+    <row r="17" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B17" s="12" t="s">
         <v>22</v>
       </c>
       <c r="C17" s="13"/>
-      <c r="D17" s="17" t="s">
+      <c r="D17" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="E17" s="17" t="s">
+      <c r="E17" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="F17" s="17" t="s">
+      <c r="F17" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="H17" s="51"/>
-    </row>
-    <row r="18" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B18" s="41" t="s">
+      <c r="H17" s="40"/>
+    </row>
+    <row r="18" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B18" s="30" t="s">
         <v>15</v>
       </c>
-      <c r="D18" s="42">
+      <c r="D18" s="31">
         <v>140000000000</v>
       </c>
-      <c r="E18" s="43">
+      <c r="E18" s="32">
         <v>1000000000</v>
       </c>
-      <c r="F18" s="43">
+      <c r="F18" s="32">
         <v>270000000</v>
       </c>
     </row>
-    <row r="19" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B19" s="30" t="s">
+    <row r="19" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B19" s="22" t="s">
         <v>10</v>
       </c>
-      <c r="C19" s="29"/>
-      <c r="D19" s="28">
+      <c r="C19" s="21"/>
+      <c r="D19" s="20">
         <v>95.17</v>
       </c>
-      <c r="E19" s="28">
+      <c r="E19" s="20">
         <v>93.41</v>
       </c>
-      <c r="F19" s="28">
+      <c r="F19" s="20">
         <v>54.22</v>
       </c>
     </row>
-    <row r="20" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B20" s="31" t="s">
+    <row r="20" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B20" s="23" t="s">
         <v>11</v>
       </c>
-      <c r="C20" s="32"/>
-      <c r="D20" s="33">
+      <c r="C20" s="24"/>
+      <c r="D20" s="25">
         <v>99.51</v>
       </c>
-      <c r="E20" s="33">
+      <c r="E20" s="25">
         <v>63.33</v>
       </c>
-      <c r="F20" s="33">
+      <c r="F20" s="25">
         <v>9.67</v>
       </c>
     </row>
-    <row r="21" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B21" s="39" t="s">
+    <row r="21" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B21" s="28" t="s">
         <v>12</v>
       </c>
-      <c r="C21" s="40"/>
-      <c r="D21" s="20">
+      <c r="C21" s="29"/>
+      <c r="D21" s="16">
         <v>90</v>
       </c>
-      <c r="E21" s="20">
+      <c r="E21" s="16">
         <v>39.57</v>
       </c>
-      <c r="F21" s="20">
+      <c r="F21" s="16">
         <v>28</v>
       </c>
     </row>
-    <row r="30" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="I30" s="47"/>
-      <c r="J30" s="47"/>
-      <c r="K30" s="47"/>
-      <c r="L30" s="47"/>
-      <c r="M30" s="47"/>
-    </row>
-    <row r="31" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="J22" s="41"/>
+    </row>
+    <row r="30" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="I30" s="36"/>
+      <c r="J30" s="36"/>
+      <c r="K30" s="36"/>
+      <c r="L30" s="36"/>
+      <c r="M30" s="36"/>
+    </row>
+    <row r="31" spans="2:13" x14ac:dyDescent="0.25">
       <c r="I31" s="2"/>
       <c r="J31" s="2"/>
       <c r="K31" s="2"/>
       <c r="L31" s="2"/>
       <c r="M31" s="2"/>
     </row>
-    <row r="32" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="32" spans="2:13" x14ac:dyDescent="0.25">
       <c r="H32" s="2"/>
       <c r="I32" s="3"/>
       <c r="J32" s="3"/>
       <c r="K32" s="3"/>
-      <c r="L32" s="45"/>
-      <c r="M32" s="45"/>
+      <c r="L32" s="34"/>
+      <c r="M32" s="34"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
calculated p-values with log transformation
</commit_message>
<xml_diff>
--- a/EvaluationMatura.xlsx
+++ b/EvaluationMatura.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\stant\Desktop\ksba\MATURA\matura\matura\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\A_118784\Desktop\matura_github\matura\matura\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE7C1119-7055-4F16-B216-FA251BFC199E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2239D055-36ED-4BEE-9AD4-07DE9E0224AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{1FCD806C-C0A2-4BF2-8B1F-847BB30B9D6D}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{1FCD806C-C0A2-4BF2-8B1F-847BB30B9D6D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -120,12 +120,13 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="5">
+  <numFmts count="6">
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="164" formatCode="0.000000"/>
     <numFmt numFmtId="165" formatCode="0.0000000"/>
     <numFmt numFmtId="166" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="172" formatCode="0.000"/>
+    <numFmt numFmtId="167" formatCode="0.000"/>
+    <numFmt numFmtId="171" formatCode="0.000000000"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -389,7 +390,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="55">
+  <cellXfs count="56">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -480,7 +481,7 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="172" fontId="0" fillId="7" borderId="15" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="167" fontId="0" fillId="7" borderId="15" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -511,6 +512,7 @@
     <xf numFmtId="164" fontId="1" fillId="3" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -854,27 +856,27 @@
   <dimension ref="B2:AD32"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J20" sqref="J20:J21"/>
+      <selection activeCell="D14" sqref="D14:I14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="26.7109375" customWidth="1"/>
-    <col min="2" max="3" width="14.7109375" customWidth="1"/>
-    <col min="4" max="4" width="16.140625" customWidth="1"/>
+    <col min="1" max="1" width="26.6640625" customWidth="1"/>
+    <col min="2" max="3" width="14.6640625" customWidth="1"/>
+    <col min="4" max="4" width="16.109375" customWidth="1"/>
     <col min="5" max="5" width="15" customWidth="1"/>
-    <col min="6" max="6" width="17.42578125" customWidth="1"/>
-    <col min="7" max="7" width="17.140625" customWidth="1"/>
-    <col min="8" max="8" width="18.28515625" customWidth="1"/>
-    <col min="9" max="9" width="19.28515625" customWidth="1"/>
-    <col min="10" max="10" width="18.28515625" customWidth="1"/>
+    <col min="6" max="6" width="17.44140625" customWidth="1"/>
+    <col min="7" max="7" width="17.109375" customWidth="1"/>
+    <col min="8" max="8" width="18.33203125" customWidth="1"/>
+    <col min="9" max="9" width="19.33203125" customWidth="1"/>
+    <col min="10" max="10" width="18.33203125" customWidth="1"/>
     <col min="11" max="11" width="17" customWidth="1"/>
-    <col min="12" max="12" width="15.28515625" customWidth="1"/>
-    <col min="13" max="13" width="15.140625" customWidth="1"/>
-    <col min="14" max="14" width="15.7109375" customWidth="1"/>
+    <col min="12" max="12" width="15.33203125" customWidth="1"/>
+    <col min="13" max="13" width="15.109375" customWidth="1"/>
+    <col min="14" max="14" width="15.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:30" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:30" x14ac:dyDescent="0.3">
       <c r="D2" s="33"/>
       <c r="E2" s="33"/>
       <c r="F2" s="33"/>
@@ -884,7 +886,7 @@
       <c r="J2" s="33"/>
       <c r="K2" s="33"/>
     </row>
-    <row r="4" spans="2:30" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:30" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B4" s="12" t="s">
         <v>20</v>
       </c>
@@ -908,7 +910,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="2:30" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:30" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B5" s="5" t="s">
         <v>0</v>
       </c>
@@ -947,7 +949,7 @@
       <c r="AB5" s="1"/>
       <c r="AC5" s="1"/>
     </row>
-    <row r="6" spans="2:30" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:30" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B6" s="5" t="s">
         <v>7</v>
       </c>
@@ -991,7 +993,7 @@
       <c r="AB6" s="1"/>
       <c r="AC6" s="1"/>
     </row>
-    <row r="7" spans="2:30" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:30" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B7" s="5" t="s">
         <v>8</v>
       </c>
@@ -1032,7 +1034,7 @@
       <c r="AB7" s="1"/>
       <c r="AC7" s="1"/>
     </row>
-    <row r="8" spans="2:30" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:30" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B8" s="6" t="s">
         <v>1</v>
       </c>
@@ -1074,7 +1076,7 @@
       <c r="AC8" s="3"/>
       <c r="AD8" s="3"/>
     </row>
-    <row r="9" spans="2:30" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:30" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B9" s="6" t="s">
         <v>2</v>
       </c>
@@ -1116,7 +1118,7 @@
       <c r="AC9" s="3"/>
       <c r="AD9" s="3"/>
     </row>
-    <row r="10" spans="2:30" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:30" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B10" s="26" t="s">
         <v>3</v>
       </c>
@@ -1158,7 +1160,7 @@
       <c r="AC10" s="3"/>
       <c r="AD10" s="3"/>
     </row>
-    <row r="11" spans="2:30" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:30" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B11" s="26" t="s">
         <v>4</v>
       </c>
@@ -1200,7 +1202,7 @@
       <c r="AC11" s="3"/>
       <c r="AD11" s="3"/>
     </row>
-    <row r="12" spans="2:30" s="2" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:30" s="2" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B12" s="8" t="s">
         <v>5</v>
       </c>
@@ -1242,7 +1244,7 @@
       <c r="AC12" s="3"/>
       <c r="AD12" s="3"/>
     </row>
-    <row r="13" spans="2:30" s="2" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:30" s="2" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B13" s="10" t="s">
         <v>6</v>
       </c>
@@ -1284,32 +1286,40 @@
       <c r="AC13" s="3"/>
       <c r="AD13" s="3"/>
     </row>
-    <row r="14" spans="2:30" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:30" x14ac:dyDescent="0.3">
       <c r="B14" s="42" t="s">
         <v>25</v>
       </c>
       <c r="C14" s="43"/>
       <c r="D14" s="44">
-        <v>6.7999999999999999E-5</v>
+        <v>1.36392330396066E-6</v>
       </c>
       <c r="E14" s="44">
-        <v>6.2000000000000003E-5</v>
+        <v>1.6419952805587399E-6</v>
       </c>
       <c r="F14" s="44">
-        <v>4.75E-4</v>
+        <v>1.1528423584482399E-3</v>
       </c>
       <c r="G14" s="44">
-        <v>0.13441415336853399</v>
+        <v>0.14699659371128099</v>
       </c>
       <c r="H14" s="44">
-        <v>2.6458572938701601E-3</v>
+        <v>1.8587106393513699E-4</v>
       </c>
       <c r="I14" s="44">
-        <v>1.19961547549787E-2</v>
+        <v>9.7118820779140203E-4</v>
       </c>
       <c r="J14" s="30"/>
     </row>
-    <row r="17" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:30" x14ac:dyDescent="0.3">
+      <c r="D15" s="55"/>
+      <c r="E15" s="55"/>
+      <c r="F15" s="55"/>
+      <c r="G15" s="55"/>
+      <c r="H15" s="55"/>
+      <c r="I15" s="55"/>
+    </row>
+    <row r="17" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B17" s="12" t="s">
         <v>22</v>
       </c>
@@ -1325,7 +1335,7 @@
       </c>
       <c r="H17" s="40"/>
     </row>
-    <row r="18" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B18" s="30" t="s">
         <v>15</v>
       </c>
@@ -1339,7 +1349,7 @@
         <v>270000000</v>
       </c>
     </row>
-    <row r="19" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B19" s="22" t="s">
         <v>10</v>
       </c>
@@ -1354,7 +1364,7 @@
         <v>54.22</v>
       </c>
     </row>
-    <row r="20" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B20" s="23" t="s">
         <v>11</v>
       </c>
@@ -1369,7 +1379,7 @@
         <v>9.67</v>
       </c>
     </row>
-    <row r="21" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B21" s="28" t="s">
         <v>12</v>
       </c>
@@ -1384,24 +1394,24 @@
         <v>28</v>
       </c>
     </row>
-    <row r="22" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:13" x14ac:dyDescent="0.3">
       <c r="J22" s="41"/>
     </row>
-    <row r="30" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:13" x14ac:dyDescent="0.3">
       <c r="I30" s="36"/>
       <c r="J30" s="36"/>
       <c r="K30" s="36"/>
       <c r="L30" s="36"/>
       <c r="M30" s="36"/>
     </row>
-    <row r="31" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:13" x14ac:dyDescent="0.3">
       <c r="I31" s="2"/>
       <c r="J31" s="2"/>
       <c r="K31" s="2"/>
       <c r="L31" s="2"/>
       <c r="M31" s="2"/>
     </row>
-    <row r="32" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:13" x14ac:dyDescent="0.3">
       <c r="H32" s="2"/>
       <c r="I32" s="3"/>
       <c r="J32" s="3"/>

</xml_diff>

<commit_message>
finished work for today, its too late
</commit_message>
<xml_diff>
--- a/EvaluationMatura.xlsx
+++ b/EvaluationMatura.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\A_118784\Desktop\matura_github\matura\matura\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\stant\Desktop\ksba\MATURA\matura\matura\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2239D055-36ED-4BEE-9AD4-07DE9E0224AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF0E15D1-F91B-4B76-819F-9F96C63C523F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{1FCD806C-C0A2-4BF2-8B1F-847BB30B9D6D}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{1FCD806C-C0A2-4BF2-8B1F-847BB30B9D6D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -126,7 +126,7 @@
     <numFmt numFmtId="165" formatCode="0.0000000"/>
     <numFmt numFmtId="166" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="167" formatCode="0.000"/>
-    <numFmt numFmtId="171" formatCode="0.000000000"/>
+    <numFmt numFmtId="168" formatCode="0.000000000"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -512,7 +512,7 @@
     <xf numFmtId="164" fontId="1" fillId="3" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -859,24 +859,24 @@
       <selection activeCell="D14" sqref="D14:I14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="26.6640625" customWidth="1"/>
-    <col min="2" max="3" width="14.6640625" customWidth="1"/>
-    <col min="4" max="4" width="16.109375" customWidth="1"/>
+    <col min="1" max="1" width="26.7109375" customWidth="1"/>
+    <col min="2" max="3" width="14.7109375" customWidth="1"/>
+    <col min="4" max="4" width="16.140625" customWidth="1"/>
     <col min="5" max="5" width="15" customWidth="1"/>
-    <col min="6" max="6" width="17.44140625" customWidth="1"/>
-    <col min="7" max="7" width="17.109375" customWidth="1"/>
-    <col min="8" max="8" width="18.33203125" customWidth="1"/>
-    <col min="9" max="9" width="19.33203125" customWidth="1"/>
-    <col min="10" max="10" width="18.33203125" customWidth="1"/>
+    <col min="6" max="6" width="17.42578125" customWidth="1"/>
+    <col min="7" max="7" width="17.140625" customWidth="1"/>
+    <col min="8" max="8" width="18.28515625" customWidth="1"/>
+    <col min="9" max="9" width="19.28515625" customWidth="1"/>
+    <col min="10" max="10" width="18.28515625" customWidth="1"/>
     <col min="11" max="11" width="17" customWidth="1"/>
-    <col min="12" max="12" width="15.33203125" customWidth="1"/>
-    <col min="13" max="13" width="15.109375" customWidth="1"/>
-    <col min="14" max="14" width="15.6640625" customWidth="1"/>
+    <col min="12" max="12" width="15.28515625" customWidth="1"/>
+    <col min="13" max="13" width="15.140625" customWidth="1"/>
+    <col min="14" max="14" width="15.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:30" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:30" x14ac:dyDescent="0.25">
       <c r="D2" s="33"/>
       <c r="E2" s="33"/>
       <c r="F2" s="33"/>
@@ -886,7 +886,7 @@
       <c r="J2" s="33"/>
       <c r="K2" s="33"/>
     </row>
-    <row r="4" spans="2:30" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:30" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="12" t="s">
         <v>20</v>
       </c>
@@ -910,7 +910,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="2:30" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:30" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B5" s="5" t="s">
         <v>0</v>
       </c>
@@ -949,7 +949,7 @@
       <c r="AB5" s="1"/>
       <c r="AC5" s="1"/>
     </row>
-    <row r="6" spans="2:30" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:30" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B6" s="5" t="s">
         <v>7</v>
       </c>
@@ -993,7 +993,7 @@
       <c r="AB6" s="1"/>
       <c r="AC6" s="1"/>
     </row>
-    <row r="7" spans="2:30" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:30" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B7" s="5" t="s">
         <v>8</v>
       </c>
@@ -1034,7 +1034,7 @@
       <c r="AB7" s="1"/>
       <c r="AC7" s="1"/>
     </row>
-    <row r="8" spans="2:30" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:30" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B8" s="6" t="s">
         <v>1</v>
       </c>
@@ -1076,7 +1076,7 @@
       <c r="AC8" s="3"/>
       <c r="AD8" s="3"/>
     </row>
-    <row r="9" spans="2:30" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:30" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B9" s="6" t="s">
         <v>2</v>
       </c>
@@ -1118,7 +1118,7 @@
       <c r="AC9" s="3"/>
       <c r="AD9" s="3"/>
     </row>
-    <row r="10" spans="2:30" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:30" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B10" s="26" t="s">
         <v>3</v>
       </c>
@@ -1160,7 +1160,7 @@
       <c r="AC10" s="3"/>
       <c r="AD10" s="3"/>
     </row>
-    <row r="11" spans="2:30" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:30" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B11" s="26" t="s">
         <v>4</v>
       </c>
@@ -1202,7 +1202,7 @@
       <c r="AC11" s="3"/>
       <c r="AD11" s="3"/>
     </row>
-    <row r="12" spans="2:30" s="2" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="2:30" s="2" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B12" s="8" t="s">
         <v>5</v>
       </c>
@@ -1244,7 +1244,7 @@
       <c r="AC12" s="3"/>
       <c r="AD12" s="3"/>
     </row>
-    <row r="13" spans="2:30" s="2" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="2:30" s="2" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B13" s="10" t="s">
         <v>6</v>
       </c>
@@ -1286,7 +1286,7 @@
       <c r="AC13" s="3"/>
       <c r="AD13" s="3"/>
     </row>
-    <row r="14" spans="2:30" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B14" s="42" t="s">
         <v>25</v>
       </c>
@@ -1311,7 +1311,7 @@
       </c>
       <c r="J14" s="30"/>
     </row>
-    <row r="15" spans="2:30" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:30" x14ac:dyDescent="0.25">
       <c r="D15" s="55"/>
       <c r="E15" s="55"/>
       <c r="F15" s="55"/>
@@ -1319,7 +1319,7 @@
       <c r="H15" s="55"/>
       <c r="I15" s="55"/>
     </row>
-    <row r="17" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B17" s="12" t="s">
         <v>22</v>
       </c>
@@ -1335,7 +1335,7 @@
       </c>
       <c r="H17" s="40"/>
     </row>
-    <row r="18" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B18" s="30" t="s">
         <v>15</v>
       </c>
@@ -1349,7 +1349,7 @@
         <v>270000000</v>
       </c>
     </row>
-    <row r="19" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B19" s="22" t="s">
         <v>10</v>
       </c>
@@ -1364,7 +1364,7 @@
         <v>54.22</v>
       </c>
     </row>
-    <row r="20" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B20" s="23" t="s">
         <v>11</v>
       </c>
@@ -1379,7 +1379,7 @@
         <v>9.67</v>
       </c>
     </row>
-    <row r="21" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B21" s="28" t="s">
         <v>12</v>
       </c>
@@ -1394,24 +1394,24 @@
         <v>28</v>
       </c>
     </row>
-    <row r="22" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:13" x14ac:dyDescent="0.25">
       <c r="J22" s="41"/>
     </row>
-    <row r="30" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:13" x14ac:dyDescent="0.25">
       <c r="I30" s="36"/>
       <c r="J30" s="36"/>
       <c r="K30" s="36"/>
       <c r="L30" s="36"/>
       <c r="M30" s="36"/>
     </row>
-    <row r="31" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="31" spans="2:13" x14ac:dyDescent="0.25">
       <c r="I31" s="2"/>
       <c r="J31" s="2"/>
       <c r="K31" s="2"/>
       <c r="L31" s="2"/>
       <c r="M31" s="2"/>
     </row>
-    <row r="32" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="32" spans="2:13" x14ac:dyDescent="0.25">
       <c r="H32" s="2"/>
       <c r="I32" s="3"/>
       <c r="J32" s="3"/>

</xml_diff>